<commit_message>
xl fike code change
</commit_message>
<xml_diff>
--- a/teacher.html.xlsx
+++ b/teacher.html.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,16 +19,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="2">
   <si>
     <t>mjjj</t>
+  </si>
+  <si>
+    <t>hellow friend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,7 +138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,7 +173,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,23 +350,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C3:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
       <c r="C5" s="1">
         <v>1</v>
       </c>
@@ -379,7 +382,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7">
       <c r="C6" s="1">
         <v>2</v>
       </c>
@@ -390,7 +393,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7">
       <c r="C7" s="1">
         <v>3</v>
       </c>
@@ -401,7 +404,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7">
       <c r="C8" s="1">
         <v>4</v>
       </c>
@@ -412,7 +415,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7">
       <c r="C9" s="1">
         <v>5</v>
       </c>
@@ -423,7 +426,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7">
       <c r="C10" s="1">
         <v>6</v>
       </c>
@@ -434,7 +437,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7">
       <c r="C11" s="1">
         <v>7</v>
       </c>
@@ -445,7 +448,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7">
       <c r="C12" s="1">
         <v>8</v>
       </c>
@@ -456,7 +459,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7">
       <c r="C13" s="1">
         <v>9</v>
       </c>
@@ -467,7 +470,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7">
       <c r="C14" s="1">
         <v>10</v>
       </c>
@@ -478,7 +481,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:7">
       <c r="C15" s="1">
         <v>11</v>
       </c>
@@ -489,7 +492,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7">
       <c r="C16" s="1">
         <v>12</v>
       </c>
@@ -500,7 +503,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7">
       <c r="C17" s="1">
         <v>13</v>
       </c>
@@ -511,7 +514,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7">
       <c r="C18" s="1">
         <v>14</v>
       </c>
@@ -522,7 +525,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7">
       <c r="C19" s="1">
         <v>15</v>
       </c>
@@ -533,7 +536,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:7">
       <c r="C20" s="1">
         <v>16</v>
       </c>
@@ -544,63 +547,63 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:7">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:7">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:7">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:7">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>

</xml_diff>